<commit_message>
Adição do campo Ano e migração do campo Data
</commit_message>
<xml_diff>
--- a/SME.CDEP.Webapi/Modelos/planilha_acervo_arte_grafica.xlsx
+++ b/SME.CDEP.Webapi/Modelos/planilha_acervo_arte_grafica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://amcomcorp-my.sharepoint.com/personal/vinicius_nyari_amcom_com_br/Documents/CDEP/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\SME-CDEP\SME.CDEP.Webapi\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="52" documentId="8_{5F512F76-96EE-40E0-9E10-AF75CE1D773C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8B2BD24F-6AA7-40EF-B87A-A25997094631}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3A7F39-966A-4C4C-93AD-2DE7A9E2EC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Acervo Arte Gráfica" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
   <si>
     <t>Título</t>
   </si>
@@ -87,6 +87,9 @@
   </si>
   <si>
     <t>Autorização do uso de imagem</t>
+  </si>
+  <si>
+    <t>Ano</t>
   </si>
 </sst>
 </file>
@@ -139,10 +142,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -442,10 +441,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046B73FB-C87D-48E8-A7D3-9135FC71E2FD}">
-  <dimension ref="A1:Q1"/>
+  <dimension ref="A1:R1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="L1" sqref="L1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,19 +453,20 @@
     <col min="3" max="3" width="12.6328125" customWidth="1"/>
     <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="11.26953125" customWidth="1"/>
+    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,39 +483,42 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>16</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>6</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>11</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>2</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>3</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
-      <c r="Q1" t="s">
+      <c r="R1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Removendo o campo data do acervo arte gráfica
</commit_message>
<xml_diff>
--- a/SME.CDEP.Webapi/Modelos/planilha_acervo_arte_grafica.xlsx
+++ b/SME.CDEP.Webapi/Modelos/planilha_acervo_arte_grafica.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27425"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Repo\SME-CDEP\SME.CDEP.Webapi\Modelos\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB3A7F39-966A-4C4C-93AD-2DE7A9E2EC9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EAA5FAF5-FF01-4AD0-8FB2-FE77E6F3C2F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{8747D3B7-822B-4607-8FA2-705F31D0AF8F}"/>
   </bookViews>
   <sheets>
     <sheet name="Acervo Arte Gráfica" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Título</t>
   </si>
@@ -66,9 +66,6 @@
   </si>
   <si>
     <t>Procedência</t>
-  </si>
-  <si>
-    <t>Data</t>
   </si>
   <si>
     <t>Cromia</t>
@@ -145,9 +142,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -185,7 +182,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -291,7 +288,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -433,7 +430,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -441,10 +438,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{046B73FB-C87D-48E8-A7D3-9135FC71E2FD}">
-  <dimension ref="A1:R1"/>
+  <dimension ref="A1:Q1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L1" sqref="L1"/>
+      <selection activeCell="I10" sqref="I10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -454,19 +451,19 @@
     <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="11.26953125" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="11.26953125" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="27.26953125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="20.1796875" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="19.1796875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="22.1796875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="19.7265625" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="10.36328125" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="11.453125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="27.26953125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="20.1796875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="19.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="22.1796875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="19.7265625" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="11.453125" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="20.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -483,28 +480,28 @@
         <v>9</v>
       </c>
       <c r="F1" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" t="s">
+        <v>15</v>
+      </c>
+      <c r="I1" t="s">
+        <v>6</v>
+      </c>
+      <c r="J1" t="s">
         <v>10</v>
       </c>
-      <c r="H1" t="s">
-        <v>5</v>
-      </c>
-      <c r="I1" t="s">
-        <v>16</v>
-      </c>
-      <c r="J1" t="s">
-        <v>6</v>
-      </c>
       <c r="K1" t="s">
+        <v>2</v>
+      </c>
+      <c r="L1" t="s">
+        <v>3</v>
+      </c>
+      <c r="M1" t="s">
         <v>11</v>
-      </c>
-      <c r="L1" t="s">
-        <v>2</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
       </c>
       <c r="N1" t="s">
         <v>12</v>
@@ -516,9 +513,6 @@
         <v>14</v>
       </c>
       <c r="Q1" t="s">
-        <v>15</v>
-      </c>
-      <c r="R1" t="s">
         <v>1</v>
       </c>
     </row>

</xml_diff>